<commit_message>
Update Propuesta Sistema control Distribuidores.xlsx
</commit_message>
<xml_diff>
--- a/excel/Propuesta Sistema control Distribuidores.xlsx
+++ b/excel/Propuesta Sistema control Distribuidores.xlsx
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:F64"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G95" sqref="A88:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,219 +1444,391 @@
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F88" t="s">
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4" t="s">
         <v>104</v>
       </c>
+      <c r="G88" s="4"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
+      <c r="A89" s="4"/>
+      <c r="B89" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F89" t="s">
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="G89" s="4"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="1" t="s">
+      <c r="A90" s="4"/>
+      <c r="B90" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F90" t="s">
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="G90" s="4"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
+      <c r="A91" s="4"/>
+      <c r="B91" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F91" t="s">
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="4" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="1" t="s">
+      <c r="A92" s="4"/>
+      <c r="B92" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F92" t="s">
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="G92" s="4"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
+      <c r="A93" s="4"/>
+      <c r="B93" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F93" t="s">
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="G93" s="4"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="1" t="s">
+      <c r="A94" s="4"/>
+      <c r="B94" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="1" t="s">
+      <c r="A95" s="4"/>
+      <c r="B95" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="1" t="s">
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="1" t="s">
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="1" t="s">
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="4"/>
+      <c r="B105" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="1" t="s">
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+      <c r="B106" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="1" t="s">
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="4"/>
+      <c r="B109" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="1" t="s">
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+      <c r="B110" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="1" t="s">
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="4"/>
+      <c r="B113" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="1" t="s">
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="4"/>
+      <c r="B114" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="1" t="s">
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="4"/>
+      <c r="B115" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="1" t="s">
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="4"/>
+      <c r="B116" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="1" t="s">
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="4"/>
+      <c r="B117" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="1" t="s">
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="4"/>
+      <c r="B118" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="1" t="s">
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="4"/>
+      <c r="B119" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="1" t="s">
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="4"/>
+      <c r="B120" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="1" t="s">
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="1" t="s">
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="4"/>
+      <c r="B122" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="1" t="s">
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="4"/>
+      <c r="B123" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="1" t="s">
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="4"/>
+      <c r="B124" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="1" t="s">
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="4"/>
+      <c r="B125" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="1" t="s">
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="4"/>
+      <c r="B126" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="1" t="s">
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="4"/>
+      <c r="B127" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>